<commit_message>
alle peilvakken node ides and overlast
</commit_message>
<xml_diff>
--- a/peilen_peilvakken.xlsx
+++ b/peilen_peilvakken.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louiseklingen/code/MargaritaLK/rtcxdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C69AF7B-8C93-774B-A9DA-96B09CF58EC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EDD10B-5856-BA42-B108-EE0E354BFFF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{98BFC175-2896-8146-8168-2F6881D15EBF}"/>
+    <workbookView xWindow="11780" yWindow="460" windowWidth="16440" windowHeight="20540" xr2:uid="{98BFC175-2896-8146-8168-2F6881D15EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -81,13 +81,130 @@
   </si>
   <si>
     <t>03150-26</t>
+  </si>
+  <si>
+    <t>03150-40</t>
+  </si>
+  <si>
+    <t>03150-43</t>
+  </si>
+  <si>
+    <t>03150-39</t>
+  </si>
+  <si>
+    <t>03150-44</t>
+  </si>
+  <si>
+    <t>03150-50</t>
+  </si>
+  <si>
+    <t>03150-49</t>
+  </si>
+  <si>
+    <t>03150-46</t>
+  </si>
+  <si>
+    <t>03150-41</t>
+  </si>
+  <si>
+    <t>03150-33</t>
+  </si>
+  <si>
+    <t>03150-36</t>
+  </si>
+  <si>
+    <t>03150-47</t>
+  </si>
+  <si>
+    <t>03150-35</t>
+  </si>
+  <si>
+    <t>03150-45</t>
+  </si>
+  <si>
+    <t>03150-01</t>
+  </si>
+  <si>
+    <t>03150-02</t>
+  </si>
+  <si>
+    <t>03150-03</t>
+  </si>
+  <si>
+    <t>03150-07</t>
+  </si>
+  <si>
+    <t>03150-08</t>
+  </si>
+  <si>
+    <t>03150-09</t>
+  </si>
+  <si>
+    <t>03150-11</t>
+  </si>
+  <si>
+    <t>03150-12</t>
+  </si>
+  <si>
+    <t>03150-13</t>
+  </si>
+  <si>
+    <t>03150-14</t>
+  </si>
+  <si>
+    <t>03150-15</t>
+  </si>
+  <si>
+    <t>03150-16</t>
+  </si>
+  <si>
+    <t>03150-17</t>
+  </si>
+  <si>
+    <t>03150-18</t>
+  </si>
+  <si>
+    <t>03150-22</t>
+  </si>
+  <si>
+    <t>03150-25</t>
+  </si>
+  <si>
+    <t>03150-28</t>
+  </si>
+  <si>
+    <t>03150-30</t>
+  </si>
+  <si>
+    <t>03150-31</t>
+  </si>
+  <si>
+    <t>03150-32</t>
+  </si>
+  <si>
+    <t>03150-34</t>
+  </si>
+  <si>
+    <t>03150-38</t>
+  </si>
+  <si>
+    <t>03150-48</t>
+  </si>
+  <si>
+    <t>03150-51</t>
+  </si>
+  <si>
+    <t>03150-52</t>
+  </si>
+  <si>
+    <t>03350-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -441,19 +558,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F785983-5C16-DE45-863B-7A4825434E8A}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,194 +584,719 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2">
-        <v>-3.1</v>
+        <v>-2.4</v>
       </c>
       <c r="D2" s="2">
-        <v>-2.4000000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2">
-        <v>-3.1</v>
+        <v>-2.85</v>
       </c>
       <c r="D3" s="2">
-        <v>-2.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>-1.6500000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2">
-        <v>-3.1</v>
+        <v>-2.4</v>
       </c>
       <c r="D4" s="2">
-        <v>-2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>-3.9</v>
-      </c>
-      <c r="D5">
-        <v>-3.55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-3.1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>-3.4</v>
+        <v>-3.1</v>
       </c>
       <c r="D6" s="2">
-        <v>-2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>-3.4</v>
+        <v>-3.1</v>
       </c>
       <c r="D7" s="2">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>-3.4</v>
-      </c>
-      <c r="D8">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-2.75</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-1.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>-3.7</v>
-      </c>
-      <c r="D9">
-        <v>-2.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>-3.7</v>
+        <v>34</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-2.6</v>
       </c>
       <c r="D10">
-        <v>-3.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
+      <c r="B11" t="s">
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>-3.75</v>
+        <v>-3.9</v>
       </c>
       <c r="D11">
-        <v>-3.35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>-3.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2">
-        <v>-3</v>
+        <v>-1.85</v>
       </c>
       <c r="D12" s="2">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>-1.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-2.7</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-2.35</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-1.85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="C13">
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-1.45</v>
+      </c>
+      <c r="D16" s="2">
+        <v>-0.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-2.35</v>
+      </c>
+      <c r="D17" s="2">
+        <v>-1.85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="2">
+        <v>-2.15</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-1.65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-3.4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-3.4</v>
+      </c>
+      <c r="D21" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>-3.4</v>
+      </c>
+      <c r="D22">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="2">
+        <v>-2.7</v>
+      </c>
+      <c r="D23" s="2">
+        <v>-2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>-3.7</v>
+      </c>
+      <c r="D24">
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>-3.7</v>
+      </c>
+      <c r="D25">
+        <v>-3.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="2">
+        <v>-3.15</v>
+      </c>
+      <c r="D26" s="2">
+        <v>-2.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27">
         <v>-3.6</v>
       </c>
-      <c r="D13">
+      <c r="D27">
         <v>-3.4</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>-3.75</v>
+      </c>
+      <c r="D28">
+        <v>-3.35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="2">
+        <v>-3.1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="2">
+        <v>-3.3</v>
+      </c>
+      <c r="D30" s="2">
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="2">
+        <v>-3.45</v>
+      </c>
+      <c r="D31" s="2">
+        <v>-2.95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="2">
+        <v>-3.5</v>
+      </c>
+      <c r="D32" s="2">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="2">
+        <v>-3.7</v>
+      </c>
+      <c r="D33" s="2">
+        <v>-3.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="2">
+        <v>-3.7</v>
+      </c>
+      <c r="D34" s="2">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="2">
+        <v>-3.4</v>
+      </c>
+      <c r="D35" s="2">
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="2">
+        <v>-3.35</v>
+      </c>
+      <c r="D36" s="2">
+        <v>-2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="2">
+        <v>-3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="2">
+        <v>-3.7</v>
+      </c>
+      <c r="D38" s="2">
+        <v>-1.7000000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="2">
+        <v>-3.6</v>
+      </c>
+      <c r="D39" s="2">
+        <v>-3.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="2">
+        <v>-3.2</v>
+      </c>
+      <c r="D40" s="2">
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="2">
+        <v>-1.85</v>
+      </c>
+      <c r="D41" s="2">
+        <v>-1.35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="2">
+        <v>-3.05</v>
+      </c>
+      <c r="D42" s="2">
+        <v>-2.15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="2">
+        <v>-2.8</v>
+      </c>
+      <c r="D43" s="2">
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="2">
+        <v>-3.5</v>
+      </c>
+      <c r="D44" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="2">
+        <v>-3.7</v>
+      </c>
+      <c r="D45" s="2">
+        <v>-3.3000000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="2">
+        <v>-3.15</v>
+      </c>
+      <c r="D46" s="2">
+        <v>-2.3499999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="2">
+        <v>-3.7</v>
+      </c>
+      <c r="D47" s="2">
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="2">
+        <v>-3.6</v>
+      </c>
+      <c r="D48" s="2">
+        <v>-2.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="2">
+        <v>-3.2</v>
+      </c>
+      <c r="D49" s="2">
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="2">
+        <v>-3.15</v>
+      </c>
+      <c r="D50" s="2">
+        <v>-2.25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="2">
+        <v>-2.75</v>
+      </c>
+      <c r="D51" s="2">
+        <v>-2.25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="2">
+        <v>-3.4</v>
+      </c>
+      <c r="D52" s="2">
+        <v>-2.9</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D20">

</xml_diff>